<commit_message>
bug fix, endurance figmerit
</commit_message>
<xml_diff>
--- a/data/Bolometer_readings_PulseForge.xlsx
+++ b/data/Bolometer_readings_PulseForge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenetjong/Bayesian-Optimization-Ferroelectrics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9639DE55-701F-C84C-A940-9F195D01657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB3D3F-E6A9-D946-871F-AA18C1637A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26250,8 +26250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26549,7 +26549,7 @@
         <v>0.84387099208632954</v>
       </c>
       <c r="I7" s="2">
-        <v>2.6001323817483191</v>
+        <v>2.677244640050493</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -26593,7 +26593,7 @@
         <v>0.58856787583946013</v>
       </c>
       <c r="I8" s="2">
-        <v>1.3404698130255503</v>
+        <v>1.4181565912852203</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -26637,7 +26637,7 @@
         <v>1.6505236082036818</v>
       </c>
       <c r="I9" s="2">
-        <v>3.8220865188186721</v>
+        <v>3.8050528055652655</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -26681,7 +26681,7 @@
         <v>1.0744613816207331</v>
       </c>
       <c r="I10" s="2">
-        <v>3.2202096407411043</v>
+        <v>3.3348561928152627</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -26725,7 +26725,7 @@
         <v>2.4380445972106783</v>
       </c>
       <c r="I11" s="2">
-        <v>4.582419233725969</v>
+        <v>4.5351528173590028</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>

</xml_diff>